<commit_message>
Fix power of two error in length of SF12 symbol
</commit_message>
<xml_diff>
--- a/extra/rxwindow-scan-sample1.xlsx
+++ b/extra/rxwindow-scan-sample1.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmm\Documents\Arduino\sketches\rwc_nst_test\extras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmm\Documents\Arduino\sketches\rwc_nst_test\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ED371BAE-A0DA-45C1-989B-E4991F006E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824FB6FD-31A8-4C64-8022-93293A566DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26730" yWindow="660" windowWidth="22905" windowHeight="13485"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rxwindow-scan-sample1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -682,139 +690,139 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>2.181640625</c:v>
+                  <c:v>1.0908203125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2578125</c:v>
+                  <c:v>1.12890625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.333984375</c:v>
+                  <c:v>1.1669921875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.41015625</c:v>
+                  <c:v>1.205078125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4863281249999996</c:v>
+                  <c:v>1.2431640624999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5625</c:v>
+                  <c:v>1.28125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.638671875</c:v>
+                  <c:v>1.3193359375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7148437499999996</c:v>
+                  <c:v>1.3574218749999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.791015625</c:v>
+                  <c:v>1.3955078125</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8671875</c:v>
+                  <c:v>1.43359375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.9433593749999996</c:v>
+                  <c:v>1.4716796874999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.01953125</c:v>
+                  <c:v>1.509765625</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.095703125</c:v>
+                  <c:v>1.5478515625</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.171875</c:v>
+                  <c:v>1.5859375</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.248046875</c:v>
+                  <c:v>1.6240234375</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.32421875</c:v>
+                  <c:v>1.662109375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.400390625</c:v>
+                  <c:v>1.7001953125</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4765625</c:v>
+                  <c:v>1.73828125</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.552734375</c:v>
+                  <c:v>1.7763671875</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.62890625</c:v>
+                  <c:v>1.814453125</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.705078125</c:v>
+                  <c:v>1.8525390625</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.78125</c:v>
+                  <c:v>1.890625</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.857421875</c:v>
+                  <c:v>1.9287109375</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.9335937499999996</c:v>
+                  <c:v>1.9667968749999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.009765625</c:v>
+                  <c:v>2.0048828125</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.0859375</c:v>
+                  <c:v>2.04296875</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.1621093749999991</c:v>
+                  <c:v>2.0810546874999996</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.23828125</c:v>
+                  <c:v>2.119140625</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.314453125</c:v>
+                  <c:v>2.1572265625</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.390625</c:v>
+                  <c:v>2.1953125</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.466796875</c:v>
+                  <c:v>2.2333984375</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.54296875</c:v>
+                  <c:v>2.271484375</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.619140625</c:v>
+                  <c:v>2.3095703125</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.6953125</c:v>
+                  <c:v>2.34765625</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.771484375</c:v>
+                  <c:v>2.3857421875</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.84765625</c:v>
+                  <c:v>2.423828125</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.923828125</c:v>
+                  <c:v>2.4619140625</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.076171875</c:v>
+                  <c:v>2.5380859375</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.15234375</c:v>
+                  <c:v>2.576171875</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.228515625</c:v>
+                  <c:v>2.6142578125</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.3046875</c:v>
+                  <c:v>2.65234375</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.380859375</c:v>
+                  <c:v>2.6904296875</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.45703125</c:v>
+                  <c:v>2.728515625</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.533203125</c:v>
+                  <c:v>2.7666015625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3082,11 +3090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3132,8 +3140,8 @@
         <v>35.744</v>
       </c>
       <c r="F2">
-        <f>E2/16.384</f>
-        <v>2.181640625</v>
+        <f>E2/32.768</f>
+        <v>1.0908203125</v>
       </c>
       <c r="G2" s="1">
         <f>(D2-C2)/D2</f>
@@ -3160,8 +3168,8 @@
         <v>36.991999999999997</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F46" si="1">E3/16.384</f>
-        <v>2.2578125</v>
+        <f t="shared" ref="F3:F46" si="1">E3/32.768</f>
+        <v>1.12890625</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G46" si="2">(D3-C3)/D3</f>
@@ -3189,7 +3197,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>2.333984375</v>
+        <v>1.1669921875</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="2"/>
@@ -3217,7 +3225,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>2.41015625</v>
+        <v>1.205078125</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="2"/>
@@ -3245,7 +3253,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>2.4863281249999996</v>
+        <v>1.2431640624999998</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="2"/>
@@ -3273,7 +3281,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>2.5625</v>
+        <v>1.28125</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="2"/>
@@ -3301,7 +3309,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>2.638671875</v>
+        <v>1.3193359375</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="2"/>
@@ -3329,7 +3337,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>2.7148437499999996</v>
+        <v>1.3574218749999998</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="2"/>
@@ -3357,7 +3365,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>2.791015625</v>
+        <v>1.3955078125</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="2"/>
@@ -3385,7 +3393,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>2.8671875</v>
+        <v>1.43359375</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="2"/>
@@ -3413,7 +3421,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>2.9433593749999996</v>
+        <v>1.4716796874999998</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="2"/>
@@ -3441,7 +3449,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>3.01953125</v>
+        <v>1.509765625</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="2"/>
@@ -3469,7 +3477,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>3.095703125</v>
+        <v>1.5478515625</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="2"/>
@@ -3497,7 +3505,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>3.171875</v>
+        <v>1.5859375</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="2"/>
@@ -3525,7 +3533,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>3.248046875</v>
+        <v>1.6240234375</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="2"/>
@@ -3553,7 +3561,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>3.32421875</v>
+        <v>1.662109375</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="2"/>
@@ -3581,7 +3589,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>3.400390625</v>
+        <v>1.7001953125</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="2"/>
@@ -3609,7 +3617,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>3.4765625</v>
+        <v>1.73828125</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="2"/>
@@ -3637,7 +3645,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>3.552734375</v>
+        <v>1.7763671875</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="2"/>
@@ -3665,7 +3673,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>3.62890625</v>
+        <v>1.814453125</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="2"/>
@@ -3693,7 +3701,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>3.705078125</v>
+        <v>1.8525390625</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="2"/>
@@ -3721,7 +3729,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>3.78125</v>
+        <v>1.890625</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="2"/>
@@ -3749,7 +3757,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>3.857421875</v>
+        <v>1.9287109375</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="2"/>
@@ -3777,7 +3785,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>3.9335937499999996</v>
+        <v>1.9667968749999998</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="2"/>
@@ -3805,7 +3813,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>4.009765625</v>
+        <v>2.0048828125</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="2"/>
@@ -3833,7 +3841,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>4.0859375</v>
+        <v>2.04296875</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="2"/>
@@ -3861,7 +3869,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>4.1621093749999991</v>
+        <v>2.0810546874999996</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="2"/>
@@ -3889,7 +3897,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>4.23828125</v>
+        <v>2.119140625</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="2"/>
@@ -3917,7 +3925,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>4.314453125</v>
+        <v>2.1572265625</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="2"/>
@@ -3945,7 +3953,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>4.390625</v>
+        <v>2.1953125</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="2"/>
@@ -3973,7 +3981,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>4.466796875</v>
+        <v>2.2333984375</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="2"/>
@@ -4001,7 +4009,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>4.54296875</v>
+        <v>2.271484375</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="2"/>
@@ -4029,7 +4037,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>4.619140625</v>
+        <v>2.3095703125</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="2"/>
@@ -4057,7 +4065,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>4.6953125</v>
+        <v>2.34765625</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="2"/>
@@ -4085,7 +4093,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>4.771484375</v>
+        <v>2.3857421875</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" si="2"/>
@@ -4113,7 +4121,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>4.84765625</v>
+        <v>2.423828125</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="2"/>
@@ -4141,7 +4149,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>4.923828125</v>
+        <v>2.4619140625</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="2"/>
@@ -4169,7 +4177,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="2"/>
@@ -4197,7 +4205,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>5.076171875</v>
+        <v>2.5380859375</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="2"/>
@@ -4225,7 +4233,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="1"/>
-        <v>5.15234375</v>
+        <v>2.576171875</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" si="2"/>
@@ -4253,7 +4261,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="1"/>
-        <v>5.228515625</v>
+        <v>2.6142578125</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="2"/>
@@ -4281,7 +4289,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="1"/>
-        <v>5.3046875</v>
+        <v>2.65234375</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="2"/>
@@ -4309,7 +4317,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="1"/>
-        <v>5.380859375</v>
+        <v>2.6904296875</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="2"/>
@@ -4337,7 +4345,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>5.45703125</v>
+        <v>2.728515625</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="2"/>
@@ -4365,7 +4373,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="1"/>
-        <v>5.533203125</v>
+        <v>2.7666015625</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="2"/>

</xml_diff>